<commit_message>
Separation of qa and stg script
</commit_message>
<xml_diff>
--- a/testdata/FCfiles/qa/ManageProducts/ManageProducts.xlsx
+++ b/testdata/FCfiles/qa/ManageProducts/ManageProducts.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="330" uniqueCount="304">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="336" uniqueCount="310">
   <si>
     <t>Other</t>
   </si>
@@ -937,6 +937,24 @@
   </si>
   <si>
     <t>prodcoCw</t>
+  </si>
+  <si>
+    <t>proddjNn</t>
+  </si>
+  <si>
+    <t>prodLCHk</t>
+  </si>
+  <si>
+    <t>prodMyME</t>
+  </si>
+  <si>
+    <t>prodvJzG</t>
+  </si>
+  <si>
+    <t>prodHMEM</t>
+  </si>
+  <si>
+    <t>prodUIYs</t>
   </si>
 </sst>
 </file>
@@ -967,7 +985,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="528">
+  <fills count="540">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -3604,8 +3622,68 @@
         <fgColor indexed="9"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="532">
+  <borders count="544">
     <border>
       <left/>
       <right/>
@@ -5620,11 +5698,53 @@
       <top style="thin"/>
       <bottom style="thin"/>
     </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="283">
+  <cellXfs count="289">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyBorder="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="2" fillId="0" fontId="2" numFmtId="0" xfId="0">
@@ -5935,7 +6055,13 @@
     <xf applyBorder="true" applyFill="true" borderId="525" fillId="521" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyBorder="true" applyFill="true" borderId="527" fillId="523" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyBorder="true" applyFill="true" borderId="529" fillId="525" fontId="0" numFmtId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="527" borderId="531" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf applyBorder="true" applyFill="true" borderId="531" fillId="527" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="533" fillId="529" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="535" fillId="531" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="537" fillId="533" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="539" fillId="535" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="541" fillId="537" fontId="0" numFmtId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="539" borderId="543" xfId="0" applyFill="true" applyBorder="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle builtinId="0" name="Normal" xfId="0"/>
@@ -6305,8 +6431,8 @@
       <c r="A2" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="B2" s="282" t="s">
-        <v>303</v>
+      <c r="B2" s="288" t="s">
+        <v>309</v>
       </c>
       <c r="C2" s="7" t="s">
         <v>17</v>
@@ -6343,8 +6469,8 @@
       <c r="A3" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="B3" s="269" t="s">
-        <v>290</v>
+      <c r="B3" s="283" t="s">
+        <v>304</v>
       </c>
       <c r="C3" s="7" t="s">
         <v>17</v>
@@ -6437,8 +6563,8 @@
       <c r="A5" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="B5" s="270" t="s">
-        <v>291</v>
+      <c r="B5" s="284" t="s">
+        <v>305</v>
       </c>
       <c r="C5" s="7" t="s">
         <v>17</v>

</xml_diff>

<commit_message>
changes made against staging and qa failures
</commit_message>
<xml_diff>
--- a/testdata/FCfiles/qa/ManageProducts/ManageProducts.xlsx
+++ b/testdata/FCfiles/qa/ManageProducts/ManageProducts.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="340" uniqueCount="314">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="341" uniqueCount="315">
   <si>
     <t>Other</t>
   </si>
@@ -967,6 +967,9 @@
   </si>
   <si>
     <t>prodRuXj</t>
+  </si>
+  <si>
+    <t>prodVwWf</t>
   </si>
 </sst>
 </file>
@@ -997,7 +1000,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="548">
+  <fills count="550">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -3734,8 +3737,18 @@
         <fgColor indexed="9"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="552">
+  <borders count="554">
     <border>
       <left/>
       <right/>
@@ -5820,11 +5833,18 @@
       <top style="thin"/>
       <bottom style="thin"/>
     </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="293">
+  <cellXfs count="294">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyBorder="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="2" fillId="0" fontId="2" numFmtId="0" xfId="0">
@@ -6145,7 +6165,8 @@
     <xf applyBorder="true" applyFill="true" borderId="545" fillId="541" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyBorder="true" applyFill="true" borderId="547" fillId="543" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyBorder="true" applyFill="true" borderId="549" fillId="545" fontId="0" numFmtId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="547" borderId="551" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf applyBorder="true" applyFill="true" borderId="551" fillId="547" fontId="0" numFmtId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="549" borderId="553" xfId="0" applyFill="true" applyBorder="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle builtinId="0" name="Normal" xfId="0"/>
@@ -6515,8 +6536,8 @@
       <c r="A2" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="B2" s="292" t="s">
-        <v>313</v>
+      <c r="B2" s="293" t="s">
+        <v>314</v>
       </c>
       <c r="C2" s="7" t="s">
         <v>17</v>

</xml_diff>

<commit_message>
Reroute test data update
</commit_message>
<xml_diff>
--- a/testdata/FCfiles/qa/ManageProducts/ManageProducts.xlsx
+++ b/testdata/FCfiles/qa/ManageProducts/ManageProducts.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="364" uniqueCount="338">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="370" uniqueCount="344">
   <si>
     <t>Other</t>
   </si>
@@ -1039,6 +1039,24 @@
   </si>
   <si>
     <t>prodhUwz</t>
+  </si>
+  <si>
+    <t>prodXTCt</t>
+  </si>
+  <si>
+    <t>prodJWne</t>
+  </si>
+  <si>
+    <t>prodZLXo</t>
+  </si>
+  <si>
+    <t>prodFDok</t>
+  </si>
+  <si>
+    <t>prodplVC</t>
+  </si>
+  <si>
+    <t>prodQPJL</t>
   </si>
 </sst>
 </file>
@@ -1069,7 +1087,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="596">
+  <fills count="608">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -4046,8 +4064,68 @@
         <fgColor indexed="9"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="600">
+  <borders count="612">
     <border>
       <left/>
       <right/>
@@ -6300,11 +6378,53 @@
       <top style="thin"/>
       <bottom style="thin"/>
     </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="317">
+  <cellXfs count="323">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyBorder="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="2" fillId="0" fontId="2" numFmtId="0" xfId="0">
@@ -6649,7 +6769,13 @@
     <xf applyBorder="true" applyFill="true" borderId="593" fillId="589" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyBorder="true" applyFill="true" borderId="595" fillId="591" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyBorder="true" applyFill="true" borderId="597" fillId="593" fontId="0" numFmtId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="595" borderId="599" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf applyBorder="true" applyFill="true" borderId="599" fillId="595" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="601" fillId="597" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="603" fillId="599" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="605" fillId="601" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="607" fillId="603" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="609" fillId="605" fontId="0" numFmtId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="607" borderId="611" xfId="0" applyFill="true" applyBorder="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle builtinId="0" name="Normal" xfId="0"/>
@@ -7019,8 +7145,8 @@
       <c r="A2" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="B2" s="316" t="s">
-        <v>337</v>
+      <c r="B2" s="322" t="s">
+        <v>343</v>
       </c>
       <c r="C2" s="7" t="s">
         <v>17</v>
@@ -7057,8 +7183,8 @@
       <c r="A3" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="B3" s="306" t="s">
-        <v>327</v>
+      <c r="B3" s="317" t="s">
+        <v>338</v>
       </c>
       <c r="C3" s="7" t="s">
         <v>17</v>
@@ -7151,8 +7277,8 @@
       <c r="A5" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="B5" s="307" t="s">
-        <v>328</v>
+      <c r="B5" s="318" t="s">
+        <v>339</v>
       </c>
       <c r="C5" s="7" t="s">
         <v>17</v>

</xml_diff>

<commit_message>
Test script fixes for quick quote.
</commit_message>
<xml_diff>
--- a/testdata/FCfiles/qa/ManageProducts/ManageProducts.xlsx
+++ b/testdata/FCfiles/qa/ManageProducts/ManageProducts.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="370" uniqueCount="344">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="386" uniqueCount="360">
   <si>
     <t>Other</t>
   </si>
@@ -1057,6 +1057,54 @@
   </si>
   <si>
     <t>prodQPJL</t>
+  </si>
+  <si>
+    <t>prodJTyi</t>
+  </si>
+  <si>
+    <t>prodjBMF</t>
+  </si>
+  <si>
+    <t>prodxtZs</t>
+  </si>
+  <si>
+    <t>prodpGtu</t>
+  </si>
+  <si>
+    <t>prodtnWT</t>
+  </si>
+  <si>
+    <t>prodItJB</t>
+  </si>
+  <si>
+    <t>prodRqgZ</t>
+  </si>
+  <si>
+    <t>prodZwOc</t>
+  </si>
+  <si>
+    <t>prodcIya</t>
+  </si>
+  <si>
+    <t>prodXMEJ</t>
+  </si>
+  <si>
+    <t>prodKvHI</t>
+  </si>
+  <si>
+    <t>prodFWlv</t>
+  </si>
+  <si>
+    <t>prodbGIP</t>
+  </si>
+  <si>
+    <t>prodJLRx</t>
+  </si>
+  <si>
+    <t>prodNCCF</t>
+  </si>
+  <si>
+    <t>prodBaYp</t>
   </si>
 </sst>
 </file>
@@ -1087,7 +1135,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="608">
+  <fills count="640">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -4124,8 +4172,168 @@
         <fgColor indexed="9"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="612">
+  <borders count="644">
     <border>
       <left/>
       <right/>
@@ -6420,11 +6628,123 @@
       <top style="thin"/>
       <bottom style="thin"/>
     </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="323">
+  <cellXfs count="339">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyBorder="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="2" fillId="0" fontId="2" numFmtId="0" xfId="0">
@@ -6775,7 +7095,23 @@
     <xf applyBorder="true" applyFill="true" borderId="605" fillId="601" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyBorder="true" applyFill="true" borderId="607" fillId="603" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyBorder="true" applyFill="true" borderId="609" fillId="605" fontId="0" numFmtId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="607" borderId="611" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf applyBorder="true" applyFill="true" borderId="611" fillId="607" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="613" fillId="609" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="615" fillId="611" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="617" fillId="613" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="619" fillId="615" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="621" fillId="617" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="623" fillId="619" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="625" fillId="621" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="627" fillId="623" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="629" fillId="625" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="631" fillId="627" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="633" fillId="629" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="635" fillId="631" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="637" fillId="633" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="639" fillId="635" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="641" fillId="637" fontId="0" numFmtId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="639" borderId="643" xfId="0" applyFill="true" applyBorder="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle builtinId="0" name="Normal" xfId="0"/>
@@ -7145,8 +7481,8 @@
       <c r="A2" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="B2" s="322" t="s">
-        <v>343</v>
+      <c r="B2" s="338" t="s">
+        <v>359</v>
       </c>
       <c r="C2" s="7" t="s">
         <v>17</v>
@@ -7183,8 +7519,8 @@
       <c r="A3" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="B3" s="317" t="s">
-        <v>338</v>
+      <c r="B3" s="333" t="s">
+        <v>354</v>
       </c>
       <c r="C3" s="7" t="s">
         <v>17</v>
@@ -7277,8 +7613,8 @@
       <c r="A5" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="B5" s="318" t="s">
-        <v>339</v>
+      <c r="B5" s="334" t="s">
+        <v>355</v>
       </c>
       <c r="C5" s="7" t="s">
         <v>17</v>

</xml_diff>

<commit_message>
classic view check addition and order date selection code update
</commit_message>
<xml_diff>
--- a/testdata/FCfiles/qa/ManageProducts/ManageProducts.xlsx
+++ b/testdata/FCfiles/qa/ManageProducts/ManageProducts.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="396" uniqueCount="370">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="406" uniqueCount="380">
   <si>
     <t>Other</t>
   </si>
@@ -1135,6 +1135,36 @@
   </si>
   <si>
     <t>prodIfXf</t>
+  </si>
+  <si>
+    <t>prodwDCe</t>
+  </si>
+  <si>
+    <t>proddbyu</t>
+  </si>
+  <si>
+    <t>prodkiZT</t>
+  </si>
+  <si>
+    <t>prodYrxj</t>
+  </si>
+  <si>
+    <t>prodUnCx</t>
+  </si>
+  <si>
+    <t>prodqZYn</t>
+  </si>
+  <si>
+    <t>prodClbw</t>
+  </si>
+  <si>
+    <t>prodFeJw</t>
+  </si>
+  <si>
+    <t>prodEbBW</t>
+  </si>
+  <si>
+    <t>prodEsCE</t>
   </si>
 </sst>
 </file>
@@ -1165,7 +1195,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="660">
+  <fills count="680">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -4462,8 +4492,108 @@
         <fgColor indexed="9"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="664">
+  <borders count="684">
     <border>
       <left/>
       <right/>
@@ -6940,11 +7070,81 @@
       <top style="thin"/>
       <bottom style="thin"/>
     </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="349">
+  <cellXfs count="359">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyBorder="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="2" fillId="0" fontId="2" numFmtId="0" xfId="0">
@@ -7321,7 +7521,17 @@
     <xf applyBorder="true" applyFill="true" borderId="657" fillId="653" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyBorder="true" applyFill="true" borderId="659" fillId="655" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyBorder="true" applyFill="true" borderId="661" fillId="657" fontId="0" numFmtId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="659" borderId="663" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf applyBorder="true" applyFill="true" borderId="663" fillId="659" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="665" fillId="661" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="667" fillId="663" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="669" fillId="665" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="671" fillId="667" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="673" fillId="669" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="675" fillId="671" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="677" fillId="673" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="679" fillId="675" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="681" fillId="677" fontId="0" numFmtId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="679" borderId="683" xfId="0" applyFill="true" applyBorder="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle builtinId="0" name="Normal" xfId="0"/>
@@ -7691,8 +7901,8 @@
       <c r="A2" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="B2" s="348" t="s">
-        <v>369</v>
+      <c r="B2" s="358" t="s">
+        <v>379</v>
       </c>
       <c r="C2" s="7" t="s">
         <v>17</v>
@@ -7729,8 +7939,8 @@
       <c r="A3" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="B3" s="343" t="s">
-        <v>364</v>
+      <c r="B3" s="355" t="s">
+        <v>376</v>
       </c>
       <c r="C3" s="7" t="s">
         <v>17</v>
@@ -7823,8 +8033,8 @@
       <c r="A5" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="B5" s="344" t="s">
-        <v>365</v>
+      <c r="B5" s="356" t="s">
+        <v>377</v>
       </c>
       <c r="C5" s="7" t="s">
         <v>17</v>

</xml_diff>

<commit_message>
product billing xml update
</commit_message>
<xml_diff>
--- a/testdata/FCfiles/qa/ManageProducts/ManageProducts.xlsx
+++ b/testdata/FCfiles/qa/ManageProducts/ManageProducts.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="464" uniqueCount="438">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="465" uniqueCount="439">
   <si>
     <t>Other</t>
   </si>
@@ -1339,6 +1339,9 @@
   </si>
   <si>
     <t>prodoilI</t>
+  </si>
+  <si>
+    <t>prodXcdn</t>
   </si>
 </sst>
 </file>
@@ -1369,7 +1372,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="796">
+  <fills count="798">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -5346,8 +5349,18 @@
         <fgColor indexed="9"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="800">
+  <borders count="802">
     <border>
       <left/>
       <right/>
@@ -8300,11 +8313,18 @@
       <top style="thin"/>
       <bottom style="thin"/>
     </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="417">
+  <cellXfs count="418">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyBorder="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="2" fillId="0" fontId="2" numFmtId="0" xfId="0">
@@ -8749,7 +8769,8 @@
     <xf applyBorder="true" applyFill="true" borderId="793" fillId="789" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyBorder="true" applyFill="true" borderId="795" fillId="791" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyBorder="true" applyFill="true" borderId="797" fillId="793" fontId="0" numFmtId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="795" borderId="799" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf applyBorder="true" applyFill="true" borderId="799" fillId="795" fontId="0" numFmtId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="797" borderId="801" xfId="0" applyFill="true" applyBorder="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle builtinId="0" name="Normal" xfId="0"/>
@@ -9119,8 +9140,8 @@
       <c r="A2" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="B2" s="416" t="s">
-        <v>437</v>
+      <c r="B2" s="417" t="s">
+        <v>438</v>
       </c>
       <c r="C2" s="7" t="s">
         <v>17</v>

</xml_diff>

<commit_message>
Updated view manage order script
</commit_message>
<xml_diff>
--- a/testdata/FCfiles/qa/ManageProducts/ManageProducts.xlsx
+++ b/testdata/FCfiles/qa/ManageProducts/ManageProducts.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="465" uniqueCount="439">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="474" uniqueCount="448">
   <si>
     <t>Other</t>
   </si>
@@ -1342,6 +1342,33 @@
   </si>
   <si>
     <t>prodXcdn</t>
+  </si>
+  <si>
+    <t>prodTzJf</t>
+  </si>
+  <si>
+    <t>prodCAFh</t>
+  </si>
+  <si>
+    <t>prodmDon</t>
+  </si>
+  <si>
+    <t>prodzINb</t>
+  </si>
+  <si>
+    <t>prodrpbv</t>
+  </si>
+  <si>
+    <t>prodqGOY</t>
+  </si>
+  <si>
+    <t>prodcUZX</t>
+  </si>
+  <si>
+    <t>prodQyhi</t>
+  </si>
+  <si>
+    <t>prodAqci</t>
   </si>
 </sst>
 </file>
@@ -1372,7 +1399,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="798">
+  <fills count="816">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -5359,8 +5386,98 @@
         <fgColor indexed="9"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="802">
+  <borders count="820">
     <border>
       <left/>
       <right/>
@@ -8320,11 +8437,74 @@
       <top style="thin"/>
       <bottom style="thin"/>
     </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="418">
+  <cellXfs count="427">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyBorder="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="2" fillId="0" fontId="2" numFmtId="0" xfId="0">
@@ -8770,7 +8950,16 @@
     <xf applyBorder="true" applyFill="true" borderId="795" fillId="791" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyBorder="true" applyFill="true" borderId="797" fillId="793" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyBorder="true" applyFill="true" borderId="799" fillId="795" fontId="0" numFmtId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="797" borderId="801" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf applyBorder="true" applyFill="true" borderId="801" fillId="797" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="803" fillId="799" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="805" fillId="801" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="807" fillId="803" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="809" fillId="805" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="811" fillId="807" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="813" fillId="809" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="815" fillId="811" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="817" fillId="813" fontId="0" numFmtId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="815" borderId="819" xfId="0" applyFill="true" applyBorder="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle builtinId="0" name="Normal" xfId="0"/>
@@ -9140,8 +9329,8 @@
       <c r="A2" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="B2" s="417" t="s">
-        <v>438</v>
+      <c r="B2" s="426" t="s">
+        <v>447</v>
       </c>
       <c r="C2" s="7" t="s">
         <v>17</v>
@@ -9178,8 +9367,8 @@
       <c r="A3" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="B3" s="410" t="s">
-        <v>431</v>
+      <c r="B3" s="422" t="s">
+        <v>443</v>
       </c>
       <c r="C3" s="7" t="s">
         <v>17</v>
@@ -9272,8 +9461,8 @@
       <c r="A5" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="B5" s="405" t="s">
-        <v>426</v>
+      <c r="B5" s="423" t="s">
+        <v>444</v>
       </c>
       <c r="C5" s="7" t="s">
         <v>17</v>

</xml_diff>

<commit_message>
Addition of manage claims phase2 scripts and some other scripts creation
</commit_message>
<xml_diff>
--- a/testdata/FCfiles/qa/ManageProducts/ManageProducts.xlsx
+++ b/testdata/FCfiles/qa/ManageProducts/ManageProducts.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="474" uniqueCount="448">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="483" uniqueCount="457">
   <si>
     <t>Other</t>
   </si>
@@ -1369,6 +1369,33 @@
   </si>
   <si>
     <t>prodAqci</t>
+  </si>
+  <si>
+    <t>prodLlpT</t>
+  </si>
+  <si>
+    <t>prodHpow</t>
+  </si>
+  <si>
+    <t>prodPsNL</t>
+  </si>
+  <si>
+    <t>prodsEkE</t>
+  </si>
+  <si>
+    <t>prodZSlL</t>
+  </si>
+  <si>
+    <t>produpvU</t>
+  </si>
+  <si>
+    <t>prodWYUH</t>
+  </si>
+  <si>
+    <t>prodxYkB</t>
+  </si>
+  <si>
+    <t>proddZjB</t>
   </si>
 </sst>
 </file>
@@ -1399,7 +1426,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="816">
+  <fills count="834">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -5476,8 +5503,98 @@
         <fgColor indexed="9"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="820">
+  <borders count="838">
     <border>
       <left/>
       <right/>
@@ -8500,11 +8617,74 @@
       <top style="thin"/>
       <bottom style="thin"/>
     </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="427">
+  <cellXfs count="436">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyBorder="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="2" fillId="0" fontId="2" numFmtId="0" xfId="0">
@@ -8959,7 +9139,16 @@
     <xf applyBorder="true" applyFill="true" borderId="813" fillId="809" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyBorder="true" applyFill="true" borderId="815" fillId="811" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyBorder="true" applyFill="true" borderId="817" fillId="813" fontId="0" numFmtId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="815" borderId="819" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf applyBorder="true" applyFill="true" borderId="819" fillId="815" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="821" fillId="817" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="823" fillId="819" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="825" fillId="821" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="827" fillId="823" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="829" fillId="825" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="831" fillId="827" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="833" fillId="829" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="835" fillId="831" fontId="0" numFmtId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="833" borderId="837" xfId="0" applyFill="true" applyBorder="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle builtinId="0" name="Normal" xfId="0"/>
@@ -9329,8 +9518,8 @@
       <c r="A2" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="B2" s="426" t="s">
-        <v>447</v>
+      <c r="B2" s="434" t="s">
+        <v>455</v>
       </c>
       <c r="C2" s="7" t="s">
         <v>17</v>
@@ -9367,8 +9556,8 @@
       <c r="A3" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="B3" s="422" t="s">
-        <v>443</v>
+      <c r="B3" s="435" t="s">
+        <v>456</v>
       </c>
       <c r="C3" s="7" t="s">
         <v>17</v>
@@ -9461,8 +9650,8 @@
       <c r="A5" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="B5" s="423" t="s">
-        <v>444</v>
+      <c r="B5" s="432" t="s">
+        <v>453</v>
       </c>
       <c r="C5" s="7" t="s">
         <v>17</v>

</xml_diff>

<commit_message>
Addition of Customer PO Validation and Manage Claims Phase 2
</commit_message>
<xml_diff>
--- a/testdata/FCfiles/qa/ManageProducts/ManageProducts.xlsx
+++ b/testdata/FCfiles/qa/ManageProducts/ManageProducts.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="483" uniqueCount="457">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="484" uniqueCount="458">
   <si>
     <t>Other</t>
   </si>
@@ -1396,6 +1396,9 @@
   </si>
   <si>
     <t>proddZjB</t>
+  </si>
+  <si>
+    <t>prodearC</t>
   </si>
 </sst>
 </file>
@@ -1426,7 +1429,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="834">
+  <fills count="836">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -5593,8 +5596,18 @@
         <fgColor indexed="9"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="838">
+  <borders count="840">
     <border>
       <left/>
       <right/>
@@ -8680,11 +8693,18 @@
       <top style="thin"/>
       <bottom style="thin"/>
     </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="436">
+  <cellXfs count="437">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyBorder="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="2" fillId="0" fontId="2" numFmtId="0" xfId="0">
@@ -9148,7 +9168,8 @@
     <xf applyBorder="true" applyFill="true" borderId="831" fillId="827" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyBorder="true" applyFill="true" borderId="833" fillId="829" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyBorder="true" applyFill="true" borderId="835" fillId="831" fontId="0" numFmtId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="833" borderId="837" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf applyBorder="true" applyFill="true" borderId="837" fillId="833" fontId="0" numFmtId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="835" borderId="839" xfId="0" applyFill="true" applyBorder="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle builtinId="0" name="Normal" xfId="0"/>
@@ -9556,8 +9577,8 @@
       <c r="A3" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="B3" s="435" t="s">
-        <v>456</v>
+      <c r="B3" s="436" t="s">
+        <v>457</v>
       </c>
       <c r="C3" s="7" t="s">
         <v>17</v>

</xml_diff>